<commit_message>
Add new colums for tallysheet (volumetric, shipperrefno & receiverrefno)
Related Work Items: #6213
</commit_message>
<xml_diff>
--- a/web/Content/Files/tallysheet_format_template.xlsx
+++ b/web/Content/Files/tallysheet_format_template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Item No.</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>Item Description</t>
+  </si>
+  <si>
+    <t>Volumetric Weight kg</t>
+  </si>
+  <si>
+    <t>Receiver Alternative Contact Number</t>
+  </si>
+  <si>
+    <t>Shipper Reference Number</t>
+  </si>
+  <si>
+    <t>Receiver Reference Number</t>
   </si>
 </sst>
 </file>
@@ -407,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -421,11 +433,14 @@
     <col min="5" max="5" width="50.77734375" style="4" customWidth="1"/>
     <col min="6" max="6" width="18.77734375" style="4" customWidth="1"/>
     <col min="7" max="7" width="22.77734375" style="4" customWidth="1"/>
-    <col min="8" max="11" width="13.77734375" style="6" customWidth="1"/>
-    <col min="12" max="12" width="18.77734375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="31.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="13.77734375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="18.77734375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="18.77734375" style="4" customWidth="1"/>
+    <col min="15" max="16" width="23.77734375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -447,20 +462,32 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>